<commit_message>
fix: adjust file xlsx
</commit_message>
<xml_diff>
--- a/uploads/TESTE_PLANILHA.xlsx
+++ b/uploads/TESTE_PLANILHA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heber\OneDrive\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713C6BD2-A2EA-4B52-A1D8-FC262A75E8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28537E00-F60A-4610-9CE4-0B504A890849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>description</t>
   </si>
@@ -48,76 +48,22 @@
     <t>Débito</t>
   </si>
   <si>
-    <t>300.28</t>
-  </si>
-  <si>
-    <t>Claudio Pontes</t>
-  </si>
-  <si>
-    <t>300.31</t>
-  </si>
-  <si>
-    <t>300.32</t>
-  </si>
-  <si>
-    <t>300.34</t>
-  </si>
-  <si>
     <t>Crédito</t>
   </si>
   <si>
-    <t>300.00</t>
-  </si>
-  <si>
-    <t>287.25</t>
-  </si>
-  <si>
-    <t>100.02</t>
-  </si>
-  <si>
-    <t>1300.29</t>
-  </si>
-  <si>
-    <t>Adele Ferreira</t>
-  </si>
-  <si>
-    <t>Eliana Vasconcelos</t>
-  </si>
-  <si>
-    <t>Caio Eduardo</t>
-  </si>
-  <si>
-    <t>Jony Freitas</t>
-  </si>
-  <si>
-    <t>Evandro Martins</t>
-  </si>
-  <si>
-    <t>Paulo Roberto</t>
-  </si>
-  <si>
-    <t>Cassia Rocha</t>
-  </si>
-  <si>
     <t>Compra de Componentes Eletrônicos</t>
   </si>
   <si>
-    <t>Manutenção de Veículo</t>
-  </si>
-  <si>
-    <t>Peças de Reposição para Equipamento de Escritório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Material de Construção para Projeto Residencial </t>
-  </si>
-  <si>
-    <t>Ferramentas e Equipamentos para Jardinagem</t>
-  </si>
-  <si>
-    <t>Livros e Materiais de Estudo</t>
-  </si>
-  <si>
-    <t>Peças de Vestuário Esportivo</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Claudio Pontes Montarr</t>
+  </si>
+  <si>
+    <t>1593345a-9e7f-449b-b1ab-c9e33a4fea6a</t>
+  </si>
+  <si>
+    <t>Adele Fonseca</t>
   </si>
 </sst>
 </file>
@@ -443,10 +389,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,10 +401,11 @@
     <col min="2" max="2" width="22.08984375" customWidth="1"/>
     <col min="3" max="3" width="19.54296875" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +421,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -485,131 +435,53 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>300.12</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>45171</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>300.12</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45172</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45173</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45174</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45175</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45176</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45177</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>